<commit_message>
Completed test automation task
</commit_message>
<xml_diff>
--- a/AdvanceTask_NUnit/AdvanceTask_NUnit/TestData/TestData.xlsx
+++ b/AdvanceTask_NUnit/AdvanceTask_NUnit/TestData/TestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IndustryConnect\AdvancedTask\Task3\AdvanceTask_NUnit\AdvanceTask_NUnit\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shiri\source\repos\Task3\AdvanceTask_NUnit\AdvanceTask_NUnit\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82D12B9D-5354-4159-9617-8F6490AFCF2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{415D79C4-E8BF-44C1-8387-ABFE829BBF62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3855" yWindow="2145" windowWidth="20550" windowHeight="11835" firstSheet="2" activeTab="8" xr2:uid="{4C82B546-A906-4170-862B-A823C28742AC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="2" xr2:uid="{4C82B546-A906-4170-862B-A823C28742AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Registration" sheetId="2" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="54">
   <si>
     <t>Title</t>
   </si>
@@ -203,6 +203,9 @@
   </si>
   <si>
     <t>Credit</t>
+  </si>
+  <si>
+    <t>I am a Test Analyst</t>
   </si>
 </sst>
 </file>
@@ -709,12 +712,25 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{211D6DFF-11BF-4C71-A5C8-0AD550E9CC42}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1071,7 +1087,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3079475B-3A66-44A9-85C2-AB95794E8424}">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:O2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated TestData and Added TeamTCs
</commit_message>
<xml_diff>
--- a/AdvanceTask_NUnit/AdvanceTask_NUnit/TestData/TestData.xlsx
+++ b/AdvanceTask_NUnit/AdvanceTask_NUnit/TestData/TestData.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Advanced_Tasks\NUnit\Task3\AdvanceTask_NUnit\AdvanceTask_NUnit\TestData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{868C3CAE-5087-45E0-9E58-4D3CC18CC98B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" firstSheet="1" activeTab="8"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Registration" sheetId="2" r:id="rId1"/>
@@ -16,13 +22,14 @@
     <sheet name="Certifications" sheetId="7" r:id="rId7"/>
     <sheet name="ShareSkills" sheetId="1" r:id="rId8"/>
     <sheet name="ManageListing" sheetId="9" r:id="rId9"/>
+    <sheet name="SearchShareSkill" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="85">
   <si>
     <t>Title</t>
   </si>
@@ -129,9 +136,6 @@
     <t>http://localhost:5000</t>
   </si>
   <si>
-    <t>Taskteam@gmail.com</t>
-  </si>
-  <si>
     <t>Task</t>
   </si>
   <si>
@@ -238,12 +242,54 @@
   </si>
   <si>
     <t>Ballet Dancer</t>
+  </si>
+  <si>
+    <t>Dance</t>
+  </si>
+  <si>
+    <t>Expert</t>
+  </si>
+  <si>
+    <t>Crochet</t>
+  </si>
+  <si>
+    <t>Intermediate</t>
+  </si>
+  <si>
+    <t>SalesforceAdministrator</t>
+  </si>
+  <si>
+    <t>Salesforce</t>
+  </si>
+  <si>
+    <t>AWS</t>
+  </si>
+  <si>
+    <t>Amazon</t>
+  </si>
+  <si>
+    <t>pooja saini</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Selenium</t>
+  </si>
+  <si>
+    <t>SearchSkill</t>
+  </si>
+  <si>
+    <t>Teamtask@gmail.com</t>
+  </si>
+  <si>
+    <t>ShareSkill</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -340,6 +386,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -634,30 +683,30 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" customWidth="1"/>
+    <col min="1" max="1" width="15.81640625" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="23.5703125" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" customWidth="1"/>
+    <col min="3" max="3" width="23.54296875" customWidth="1"/>
+    <col min="4" max="4" width="13.54296875" customWidth="1"/>
+    <col min="5" max="5" width="19.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>13</v>
       </c>
@@ -686,18 +735,18 @@
       <c r="P1" s="6"/>
       <c r="Q1" s="6"/>
     </row>
-    <row r="2" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>35</v>
+        <v>83</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>21</v>
+        <v>84</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>21</v>
@@ -705,121 +754,31 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{4E598EBD-64C3-46F4-AF78-E32C90AAEEAE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P2"/>
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3746C1A-AC46-40CB-AD76-ABFAB976D2FF}">
+  <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" customWidth="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:16" s="7" customFormat="1" ht="14.45" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-    </row>
-    <row r="2" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="B2" r:id="rId2"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="23.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" customWidth="1"/>
+    <col min="1" max="1" width="14.81640625" style="15" customWidth="1"/>
+    <col min="2" max="16384" width="8.7265625" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>23</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="B1" s="6"/>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
@@ -835,30 +794,134 @@
       <c r="O1" s="6"/>
       <c r="P1" s="6"/>
     </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A2" s="15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A3" s="15" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A4" s="15" t="s">
+        <v>79</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P1"/>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="1" max="1" width="23.54296875" customWidth="1"/>
+    <col min="2" max="2" width="19.7265625" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>25</v>
+        <v>18</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+    </row>
+    <row r="2" spans="1:16" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{07FA1943-ED52-4C3E-9A43-54E3257D949A}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="23.54296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:P1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="19.54296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
@@ -880,78 +943,27 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P1"/>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A2" sqref="A2:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.85546875" customWidth="1"/>
-    <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="21.140625" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>32</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="C1" s="6"/>
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
@@ -966,40 +978,169 @@
       <c r="O1" s="6"/>
       <c r="P1" s="6"/>
     </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A2" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A3" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:P1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="25.81640625" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="5" max="5" width="21.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:P3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.54296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A2" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="15">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A3" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" s="15">
+        <v>2022</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:R4"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" customWidth="1"/>
-    <col min="2" max="2" width="56.28515625" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" customWidth="1"/>
-    <col min="4" max="4" width="25.140625" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" customWidth="1"/>
-    <col min="6" max="6" width="19.140625" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" customWidth="1"/>
+    <col min="1" max="1" width="14.26953125" customWidth="1"/>
+    <col min="2" max="2" width="56.26953125" customWidth="1"/>
+    <col min="3" max="3" width="21.453125" customWidth="1"/>
+    <col min="4" max="4" width="25.1796875" customWidth="1"/>
+    <col min="5" max="5" width="13.1796875" customWidth="1"/>
+    <col min="6" max="6" width="19.1796875" customWidth="1"/>
+    <col min="7" max="7" width="14.7265625" customWidth="1"/>
+    <col min="8" max="8" width="15.54296875" customWidth="1"/>
     <col min="9" max="9" width="15" customWidth="1"/>
-    <col min="10" max="10" width="13.42578125" customWidth="1"/>
+    <col min="10" max="10" width="13.453125" customWidth="1"/>
     <col min="11" max="11" width="19" style="15" customWidth="1"/>
-    <col min="12" max="12" width="11.42578125" customWidth="1"/>
+    <col min="12" max="12" width="11.453125" customWidth="1"/>
     <col min="13" max="14" width="15" customWidth="1"/>
-    <col min="15" max="15" width="23.7109375" customWidth="1"/>
-    <col min="16" max="16" width="11.28515625" customWidth="1"/>
-    <col min="17" max="17" width="13.140625" customWidth="1"/>
+    <col min="15" max="15" width="23.7265625" customWidth="1"/>
+    <col min="16" max="16" width="11.26953125" customWidth="1"/>
+    <col min="17" max="17" width="13.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1031,13 +1172,13 @@
         <v>8</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L1" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="M1" s="6" t="s">
         <v>69</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>70</v>
       </c>
       <c r="N1" s="6" t="s">
         <v>9</v>
@@ -1052,30 +1193,30 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B2" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="D2" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="E2" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="G2" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="E2" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>42</v>
-      </c>
       <c r="H2" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I2" s="13">
         <v>10082024</v>
@@ -1084,19 +1225,19 @@
         <v>10092024</v>
       </c>
       <c r="K2" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="L2" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="L2" s="13" t="s">
+      <c r="M2" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="M2" s="13" t="s">
-        <v>68</v>
-      </c>
       <c r="N2" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="O2" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="P2" s="13">
         <v>10</v>
@@ -1105,7 +1246,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="C3" s="3"/>
@@ -1124,7 +1265,7 @@
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -1151,87 +1292,87 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" customWidth="1"/>
-    <col min="2" max="2" width="40.28515625" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" customWidth="1"/>
-    <col min="9" max="9" width="12.85546875" customWidth="1"/>
-    <col min="10" max="10" width="11.5703125" customWidth="1"/>
-    <col min="11" max="11" width="11.85546875" customWidth="1"/>
-    <col min="13" max="13" width="15.5703125" customWidth="1"/>
+    <col min="1" max="1" width="22.26953125" customWidth="1"/>
+    <col min="2" max="2" width="40.26953125" customWidth="1"/>
+    <col min="3" max="3" width="9.7265625" customWidth="1"/>
+    <col min="4" max="4" width="12.453125" customWidth="1"/>
+    <col min="5" max="5" width="12.26953125" customWidth="1"/>
+    <col min="6" max="6" width="12.1796875" customWidth="1"/>
+    <col min="7" max="7" width="14.1796875" customWidth="1"/>
+    <col min="8" max="8" width="15.54296875" customWidth="1"/>
+    <col min="9" max="9" width="12.81640625" customWidth="1"/>
+    <col min="10" max="10" width="11.54296875" customWidth="1"/>
+    <col min="11" max="11" width="11.81640625" customWidth="1"/>
+    <col min="13" max="13" width="15.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="C1" s="15" t="s">
+      <c r="D1" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="E1" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="F1" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="G1" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="H1" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="I1" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="J1" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="J1" s="15" t="s">
+      <c r="K1" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="K1" s="15" t="s">
+      <c r="L1" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="L1" s="15" t="s">
+      <c r="M1" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="M1" s="15" t="s">
+      <c r="N1" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="N1" s="15" t="s">
+      <c r="O1" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="O1" s="15" t="s">
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A2" s="15" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="B2" s="15" t="s">
         <v>58</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>59</v>
       </c>
       <c r="C2" s="15"/>
       <c r="D2" s="15"/>
       <c r="E2" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>

</xml_diff>

<commit_message>
Updated for more Validations
</commit_message>
<xml_diff>
--- a/AdvanceTask_NUnit/AdvanceTask_NUnit/TestData/TestData.xlsx
+++ b/AdvanceTask_NUnit/AdvanceTask_NUnit/TestData/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Advanced_Tasks\Task3\AdvanceTask_NUnit\AdvanceTask_NUnit\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F29616E-6C06-4432-BC08-4BC905E1B051}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE842718-78C9-46EA-8F9A-74BC8EBC5329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{4C82B546-A906-4170-862B-A823C28742AC}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{4C82B546-A906-4170-862B-A823C28742AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Registration" sheetId="2" r:id="rId1"/>
@@ -117,10 +117,10 @@
     <t>Selenium</t>
   </si>
   <si>
+    <t>pooja saini</t>
+  </si>
+  <si>
     <t>Testing</t>
-  </si>
-  <si>
-    <t>pooja saini</t>
   </si>
 </sst>
 </file>
@@ -567,7 +567,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4525648E-70AE-4193-B5F5-534B48D41F13}">
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -737,8 +737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18972AC6-AF1D-4ABF-9FE7-FB527247F12D}">
   <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -773,12 +773,12 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>